<commit_message>
Added a 0590.HK Model
</commit_message>
<xml_diff>
--- a/financial_models/Macro_Monitor.xlsx
+++ b/financial_models/Macro_Monitor.xlsx
@@ -1,36 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/Invest_Proc_v3/financial_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\PycharmProjects\Invest_Proc_v3\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8F27C2A-18F9-3140-9742-3B7DBF65F6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1689A017-5722-4BEF-A1C2-2B5087653480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="12690" windowHeight="7643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro" sheetId="2" r:id="rId1"/>
     <sheet name="Analysis" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029" calcOnSave="0" concurrentManualCount="16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -362,11 +351,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -374,7 +363,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -447,7 +436,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -463,20 +452,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -485,7 +474,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -494,7 +483,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -844,8 +833,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1129,14 +1118,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" customWidth="1"/>
-    <col min="3" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.46484375" customWidth="1"/>
+    <col min="2" max="2" width="47.796875" customWidth="1"/>
+    <col min="3" max="6" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>68</v>
@@ -1154,7 +1143,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>67</v>
       </c>
@@ -1169,7 +1158,7 @@
       </c>
       <c r="F3" s="46"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -1182,7 +1171,7 @@
       <c r="E4" s="52"/>
       <c r="F4" s="46"/>
     </row>
-    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.25" thickBot="1">
       <c r="B5" s="48" t="s">
         <v>72</v>
       </c>
@@ -1193,7 +1182,7 @@
       <c r="E5" s="53"/>
       <c r="F5" s="51"/>
     </row>
-    <row r="6" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="14.25" thickTop="1">
       <c r="B6" s="47" t="s">
         <v>73</v>
       </c>
@@ -1210,15 +1199,15 @@
       </c>
       <c r="F6" s="55"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="B10" s="54" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="E11" s="43"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="B12" s="5" t="s">
         <v>82</v>
       </c>
@@ -1227,7 +1216,7 @@
       </c>
       <c r="E12" s="43"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="B13" s="5" t="s">
         <v>70</v>
       </c>
@@ -1235,7 +1224,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="B15" s="5" t="s">
         <v>77</v>
       </c>
@@ -1243,7 +1232,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="B16" s="5" t="s">
         <v>78</v>
       </c>
@@ -1251,7 +1240,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" s="5" t="s">
         <v>79</v>
       </c>
@@ -1259,7 +1248,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4">
       <c r="B19" s="18" t="s">
         <v>62</v>
       </c>
@@ -1268,7 +1257,7 @@
       </c>
       <c r="D19" s="40"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" s="18" t="s">
         <v>63</v>
       </c>
@@ -1277,7 +1266,7 @@
       </c>
       <c r="D20" s="40"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="B21" s="18" t="s">
         <v>64</v>
       </c>
@@ -1311,17 +1300,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.46484375" customWidth="1"/>
+    <col min="2" max="2" width="62.46484375" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.46484375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>60</v>
@@ -1335,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>59</v>
       </c>
@@ -1348,7 +1337,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="B4" s="38" t="s">
         <v>58</v>
       </c>
@@ -1362,7 +1351,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="B5" s="34" t="s">
         <v>57</v>
       </c>
@@ -1383,7 +1372,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="31" t="s">
         <v>56</v>
@@ -1399,7 +1388,7 @@
         <v>China</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>55</v>
@@ -1409,7 +1398,7 @@
       <c r="E8" s="23"/>
       <c r="F8" s="27"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="5"/>
       <c r="B9" s="23" t="s">
         <v>54</v>
@@ -1429,7 +1418,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="5"/>
       <c r="B10" s="23" t="s">
         <v>52</v>
@@ -1449,7 +1438,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="23" t="s">
         <v>49</v>
@@ -1469,7 +1458,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>47</v>
@@ -1489,7 +1478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="5"/>
       <c r="B13" s="21" t="s">
         <v>45</v>
@@ -1511,7 +1500,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="5"/>
       <c r="B14" s="23" t="s">
         <v>44</v>
@@ -1531,7 +1520,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="5"/>
       <c r="B15" s="23" t="s">
         <v>42</v>
@@ -1551,7 +1540,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="5"/>
       <c r="B16" s="23" t="s">
         <v>40</v>
@@ -1571,7 +1560,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="5"/>
       <c r="B17" s="23" t="s">
         <v>38</v>
@@ -1591,7 +1580,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="5"/>
       <c r="B18" s="21" t="s">
         <v>36</v>
@@ -1613,7 +1602,7 @@
         <v>Cold</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="5"/>
       <c r="B19" s="23" t="s">
         <v>35</v>
@@ -1633,7 +1622,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="5"/>
       <c r="B20" s="23" t="s">
         <v>32</v>
@@ -1653,7 +1642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="5"/>
       <c r="B21" s="23" t="s">
         <v>30</v>
@@ -1673,7 +1662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="5"/>
       <c r="B22" s="23" t="s">
         <v>28</v>
@@ -1693,7 +1682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="5"/>
       <c r="B23" s="21" t="s">
         <v>26</v>
@@ -1715,7 +1704,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="5"/>
       <c r="B24" s="23" t="s">
         <v>25</v>
@@ -1735,7 +1724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="5"/>
       <c r="B25" s="23" t="s">
         <v>22</v>
@@ -1755,7 +1744,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="5"/>
       <c r="B26" s="23" t="s">
         <v>20</v>
@@ -1775,7 +1764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="5"/>
       <c r="B27" s="23" t="s">
         <v>18</v>
@@ -1795,7 +1784,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="5"/>
       <c r="B28" s="21" t="s">
         <v>15</v>
@@ -1817,7 +1806,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="5"/>
       <c r="B29" s="18" t="s">
         <v>14</v>
@@ -1839,10 +1828,10 @@
         <v>Relatively pessimistic</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="5"/>
       <c r="B31" s="7" t="s">
         <v>13</v>
@@ -1856,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>12</v>
@@ -1876,7 +1865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6">
       <c r="B33" s="5" t="s">
         <v>9</v>
       </c>
@@ -1897,7 +1886,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6">
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -1918,7 +1907,7 @@
         <v>Hot - Positive</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6">
       <c r="B35" s="5" t="s">
         <v>7</v>
       </c>
@@ -1939,7 +1928,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6">
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1960,7 +1949,7 @@
         <v>Cold - Wide</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6">
       <c r="B37" s="11" t="s">
         <v>5</v>
       </c>
@@ -1981,12 +1970,12 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6">
       <c r="B39" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6">
       <c r="B40" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updated the beta version
</commit_message>
<xml_diff>
--- a/financial_models/Macro_Monitor.xlsx
+++ b/financial_models/Macro_Monitor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/Invest_Proc_v3/financial_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\PycharmProjects\Invest_Proc_v3\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769B009A-5C20-854A-9D9C-3EEE00258D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2481DE73-5867-4B56-891C-A19647FCEE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro" sheetId="2" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="86">
   <si>
     <t>China</t>
   </si>
@@ -357,16 +346,20 @@
   <si>
     <t>NOTES:</t>
   </si>
+  <si>
+    <t>Target Return</t>
+    <phoneticPr fontId="16" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -374,7 +367,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -447,7 +440,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -463,20 +456,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -485,7 +478,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -494,7 +487,7 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -844,8 +837,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1125,18 +1118,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A061C73F-1F33-4614-90A5-D5D9D7C58056}">
   <dimension ref="A2:F21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" customWidth="1"/>
-    <col min="3" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.46484375" customWidth="1"/>
+    <col min="2" max="2" width="47.796875" customWidth="1"/>
+    <col min="3" max="6" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>68</v>
@@ -1154,7 +1147,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>67</v>
       </c>
@@ -1169,7 +1162,7 @@
       </c>
       <c r="F3" s="46"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -1182,7 +1175,7 @@
       <c r="E4" s="52"/>
       <c r="F4" s="46"/>
     </row>
-    <row r="5" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="14.25" thickBot="1">
       <c r="B5" s="48" t="s">
         <v>72</v>
       </c>
@@ -1193,7 +1186,7 @@
       <c r="E5" s="53"/>
       <c r="F5" s="51"/>
     </row>
-    <row r="6" spans="1:6" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="14.25" thickTop="1">
       <c r="B6" s="47" t="s">
         <v>73</v>
       </c>
@@ -1211,15 +1204,24 @@
       </c>
       <c r="F6" s="55"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="45">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10" s="54" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="E11" s="43"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="B12" s="5" t="s">
         <v>82</v>
       </c>
@@ -1228,7 +1230,7 @@
       </c>
       <c r="E12" s="43"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="B13" s="5" t="s">
         <v>70</v>
       </c>
@@ -1236,7 +1238,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="B15" s="5" t="s">
         <v>77</v>
       </c>
@@ -1244,7 +1246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="B16" s="5" t="s">
         <v>78</v>
       </c>
@@ -1252,7 +1254,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4">
       <c r="B17" s="5" t="s">
         <v>79</v>
       </c>
@@ -1260,7 +1262,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4">
       <c r="B19" s="18" t="s">
         <v>62</v>
       </c>
@@ -1269,7 +1271,7 @@
       </c>
       <c r="D19" s="40"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4">
       <c r="B20" s="18" t="s">
         <v>63</v>
       </c>
@@ -1278,7 +1280,7 @@
       </c>
       <c r="D20" s="40"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4">
       <c r="B21" s="18" t="s">
         <v>64</v>
       </c>
@@ -1312,17 +1314,17 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.46484375" customWidth="1"/>
+    <col min="2" max="2" width="62.46484375" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.46484375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="4"/>
       <c r="B2" s="3" t="s">
         <v>60</v>
@@ -1336,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="B3" t="s">
         <v>59</v>
       </c>
@@ -1349,7 +1351,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="B4" s="38" t="s">
         <v>58</v>
       </c>
@@ -1363,7 +1365,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="B5" s="34" t="s">
         <v>57</v>
       </c>
@@ -1384,7 +1386,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7" s="4"/>
       <c r="B7" s="31" t="s">
         <v>56</v>
@@ -1400,7 +1402,7 @@
         <v>China</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="5"/>
       <c r="B8" s="7" t="s">
         <v>55</v>
@@ -1410,7 +1412,7 @@
       <c r="E8" s="23"/>
       <c r="F8" s="27"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="5"/>
       <c r="B9" s="23" t="s">
         <v>54</v>
@@ -1430,7 +1432,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="5"/>
       <c r="B10" s="23" t="s">
         <v>52</v>
@@ -1450,7 +1452,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="23" t="s">
         <v>49</v>
@@ -1470,7 +1472,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>47</v>
@@ -1490,7 +1492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="5"/>
       <c r="B13" s="21" t="s">
         <v>45</v>
@@ -1512,7 +1514,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="5"/>
       <c r="B14" s="23" t="s">
         <v>44</v>
@@ -1532,7 +1534,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="5"/>
       <c r="B15" s="23" t="s">
         <v>42</v>
@@ -1552,7 +1554,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="5"/>
       <c r="B16" s="23" t="s">
         <v>40</v>
@@ -1572,7 +1574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="5"/>
       <c r="B17" s="23" t="s">
         <v>38</v>
@@ -1592,7 +1594,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="5"/>
       <c r="B18" s="21" t="s">
         <v>36</v>
@@ -1614,7 +1616,7 @@
         <v>Cold</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="5"/>
       <c r="B19" s="23" t="s">
         <v>35</v>
@@ -1634,7 +1636,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="5"/>
       <c r="B20" s="23" t="s">
         <v>32</v>
@@ -1654,7 +1656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="5"/>
       <c r="B21" s="23" t="s">
         <v>30</v>
@@ -1674,7 +1676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="5"/>
       <c r="B22" s="23" t="s">
         <v>28</v>
@@ -1694,7 +1696,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="5"/>
       <c r="B23" s="21" t="s">
         <v>26</v>
@@ -1716,7 +1718,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="5"/>
       <c r="B24" s="23" t="s">
         <v>25</v>
@@ -1736,7 +1738,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="5"/>
       <c r="B25" s="23" t="s">
         <v>22</v>
@@ -1756,7 +1758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="5"/>
       <c r="B26" s="23" t="s">
         <v>20</v>
@@ -1776,7 +1778,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="5"/>
       <c r="B27" s="23" t="s">
         <v>18</v>
@@ -1796,7 +1798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" s="5"/>
       <c r="B28" s="21" t="s">
         <v>15</v>
@@ -1818,7 +1820,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" s="5"/>
       <c r="B29" s="18" t="s">
         <v>14</v>
@@ -1840,10 +1842,10 @@
         <v>Relatively pessimistic</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="5"/>
       <c r="B31" s="7" t="s">
         <v>13</v>
@@ -1857,7 +1859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>12</v>
@@ -1877,7 +1879,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6">
       <c r="B33" s="5" t="s">
         <v>9</v>
       </c>
@@ -1898,7 +1900,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6">
       <c r="B34" s="5" t="s">
         <v>8</v>
       </c>
@@ -1919,7 +1921,7 @@
         <v>Hot - Positive</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6">
       <c r="B35" s="5" t="s">
         <v>7</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6">
       <c r="B36" s="5" t="s">
         <v>6</v>
       </c>
@@ -1961,7 +1963,7 @@
         <v>Cold - Wide</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6">
       <c r="B37" s="11" t="s">
         <v>5</v>
       </c>
@@ -1982,12 +1984,12 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6">
       <c r="B39" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6">
       <c r="B40" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updated the Macro data
</commit_message>
<xml_diff>
--- a/financial_models/Macro_Monitor.xlsx
+++ b/financial_models/Macro_Monitor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/Invest_Proc_v3/financial_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\PycharmProjects\Invest_Proc_v3\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044C1219-29F9-6743-B92A-0562C59A8B76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F356169B-5FB8-4B07-9340-3259B231B4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="RE" sheetId="6" r:id="rId3"/>
     <sheet name="Analysis" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentManualCount="8"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -457,11 +457,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -469,7 +469,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -544,13 +544,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -866,8 +866,8 @@
     <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1147,19 +1147,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A061C73F-1F33-4614-90A5-D5D9D7C58056}">
   <dimension ref="A2:F40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView showGridLines="0" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="22" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" style="22" customWidth="1"/>
-    <col min="3" max="6" width="20.83203125" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="22"/>
+    <col min="1" max="1" width="2.46484375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="47.796875" style="22" customWidth="1"/>
+    <col min="3" max="6" width="20.796875" style="22" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="22"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>64</v>
@@ -1177,7 +1177,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="B3" s="22" t="s">
         <v>63</v>
       </c>
@@ -1192,7 +1192,7 @@
       </c>
       <c r="F3" s="33"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="B4" s="22" t="s">
         <v>67</v>
       </c>
@@ -1205,7 +1205,7 @@
       <c r="E4" s="38"/>
       <c r="F4" s="33"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="14.25" thickBot="1">
       <c r="B5" s="44" t="s">
         <v>68</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="E5" s="39"/>
       <c r="F5" s="37"/>
     </row>
-    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="14.25" thickTop="1">
       <c r="B6" s="20" t="s">
         <v>69</v>
       </c>
@@ -1234,7 +1234,7 @@
       </c>
       <c r="F6" s="40"/>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>80</v>
@@ -1243,7 +1243,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6">
       <c r="B10" s="22" t="s">
         <v>96</v>
       </c>
@@ -1252,10 +1252,10 @@
       </c>
       <c r="E10" s="46"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="E11" s="46"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6">
       <c r="B12" s="4" t="s">
         <v>78</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6">
       <c r="B13" s="4" t="s">
         <v>66</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="B15" s="4" t="s">
         <v>73</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6">
       <c r="B16" s="4" t="s">
         <v>74</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="B17" s="4" t="s">
         <v>75</v>
       </c>
@@ -1295,13 +1295,13 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="B21" s="4" t="s">
         <v>98</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="B23" s="4" t="s">
         <v>101</v>
       </c>
@@ -1318,10 +1318,10 @@
       </c>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="D24" s="31"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="B25" s="17" t="s">
         <v>58</v>
       </c>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="D25" s="31"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="B26" s="17" t="s">
         <v>59</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="B27" s="17" t="s">
         <v>60</v>
       </c>
@@ -1346,13 +1346,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15">
       <c r="A29" s="3"/>
       <c r="B29" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="B31" s="17" t="s">
         <v>92</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:3">
       <c r="B33" s="17" t="s">
         <v>95</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:3">
       <c r="B34" s="17" t="s">
         <v>105</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:3">
       <c r="B35" s="22" t="s">
         <v>104</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:3">
       <c r="B37" s="22" t="s">
         <v>108</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:3">
       <c r="B38" s="22" t="s">
         <v>110</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:3">
       <c r="B40" s="22" t="s">
         <v>111</v>
       </c>
@@ -1439,17 +1439,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B06D35-F870-9847-BA9B-1E2F9FFBE611}">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.9"/>
   <cols>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.5" customWidth="1"/>
+    <col min="3" max="3" width="51.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" s="34" t="s">
         <v>87</v>
       </c>
@@ -1457,12 +1457,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3">
       <c r="B4" s="34" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>81</v>
       </c>
@@ -1470,12 +1470,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" s="41" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
         <v>84</v>
       </c>
@@ -1483,12 +1483,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" s="34" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3">
       <c r="B11" t="s">
         <v>90</v>
       </c>
@@ -1497,6 +1497,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" xr:uid="{BD2948D7-96D9-264F-B0D8-E6D98C96444B}"/>
     <hyperlink ref="C8" r:id="rId2" xr:uid="{00B87B71-2B64-7648-8C06-ED4B13CF1CAC}"/>
@@ -1515,14 +1516,14 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="34.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4">
       <c r="C2" s="1" t="s">
         <v>118</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1538,32 +1539,33 @@
         <v>113</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4">
       <c r="B9" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4">
       <c r="B11" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4">
       <c r="B13" t="s">
         <v>117</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{D5EB599C-0AC8-C945-97CD-4616A9DA5B5A}"/>
   </hyperlinks>
@@ -1579,17 +1581,17 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="62.5" customWidth="1"/>
-    <col min="3" max="3" width="10.5" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.46484375" customWidth="1"/>
+    <col min="2" max="2" width="62.46484375" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="10.46484375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="3"/>
       <c r="B2" s="30" t="s">
         <v>56</v>
@@ -1603,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="4"/>
       <c r="B3" s="6" t="s">
         <v>55</v>
@@ -1613,7 +1615,7 @@
       <c r="E3" s="22"/>
       <c r="F3" s="26"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="4"/>
       <c r="B4" s="22" t="s">
         <v>54</v>
@@ -1633,7 +1635,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="4"/>
       <c r="B5" s="22" t="s">
         <v>52</v>
@@ -1653,7 +1655,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" s="4"/>
       <c r="B6" s="22" t="s">
         <v>49</v>
@@ -1673,7 +1675,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>47</v>
@@ -1693,7 +1695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" s="4"/>
       <c r="B8" s="20" t="s">
         <v>45</v>
@@ -1715,7 +1717,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="4"/>
       <c r="B9" s="22" t="s">
         <v>44</v>
@@ -1735,7 +1737,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" s="4"/>
       <c r="B10" s="22" t="s">
         <v>42</v>
@@ -1755,7 +1757,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" s="4"/>
       <c r="B11" s="22" t="s">
         <v>40</v>
@@ -1775,7 +1777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="4"/>
       <c r="B12" s="22" t="s">
         <v>38</v>
@@ -1795,7 +1797,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="4"/>
       <c r="B13" s="20" t="s">
         <v>36</v>
@@ -1817,7 +1819,7 @@
         <v>Cold</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="4"/>
       <c r="B14" s="22" t="s">
         <v>35</v>
@@ -1837,7 +1839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="4"/>
       <c r="B15" s="22" t="s">
         <v>32</v>
@@ -1857,7 +1859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="4"/>
       <c r="B16" s="22" t="s">
         <v>30</v>
@@ -1877,7 +1879,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="4"/>
       <c r="B17" s="22" t="s">
         <v>28</v>
@@ -1897,7 +1899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="4"/>
       <c r="B18" s="20" t="s">
         <v>26</v>
@@ -1919,7 +1921,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="4"/>
       <c r="B19" s="22" t="s">
         <v>25</v>
@@ -1939,7 +1941,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="4"/>
       <c r="B20" s="22" t="s">
         <v>22</v>
@@ -1959,7 +1961,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="4"/>
       <c r="B21" s="22" t="s">
         <v>20</v>
@@ -1979,7 +1981,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="4"/>
       <c r="B22" s="22" t="s">
         <v>18</v>
@@ -1999,7 +2001,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="20" t="s">
         <v>15</v>
@@ -2021,7 +2023,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="4"/>
       <c r="B24" s="17" t="s">
         <v>14</v>
@@ -2043,10 +2045,10 @@
         <v>Relatively pessimistic</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="4"/>
       <c r="B26" s="6" t="s">
         <v>13</v>
@@ -2060,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" s="4"/>
       <c r="B27" s="4" t="s">
         <v>12</v>
@@ -2080,7 +2082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="B28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="B29" s="4" t="s">
         <v>8</v>
       </c>
@@ -2122,7 +2124,7 @@
         <v>Hot - Positive</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="B30" s="4" t="s">
         <v>7</v>
       </c>
@@ -2143,7 +2145,7 @@
         <v>Mixed</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="B31" s="4" t="s">
         <v>6</v>
       </c>
@@ -2164,7 +2166,7 @@
         <v>Cold - Wide</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="B32" s="10" t="s">
         <v>5</v>
       </c>
@@ -2185,12 +2187,12 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:2">
       <c r="B34" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:2">
       <c r="B35" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Updated the main calling function
</commit_message>
<xml_diff>
--- a/financial_models/Macro_Monitor.xlsx
+++ b/financial_models/Macro_Monitor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kamanl/PycharmProjects/Invest_Proc_v3/financial_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerry\PycharmProjects\Invest_Proc_v3\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D035F52-8828-3643-8EAE-F66ABE70094E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B64121-53C7-477F-B7DF-462D3B9DF65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="17115" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Macro" sheetId="2" r:id="rId1"/>
@@ -23,23 +23,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="154">
   <si>
     <t>China</t>
   </si>
@@ -324,7 +313,7 @@
   </si>
   <si>
     <t>Target Return</t>
-    <phoneticPr fontId="12" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Crude oil</t>
@@ -442,22 +431,10 @@
   </si>
   <si>
     <t>Discount Rate</t>
-    <phoneticPr fontId="12" type="noConversion"/>
+    <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
     <t>Forex</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>CNY</t>
-  </si>
-  <si>
-    <t>HKD</t>
-  </si>
-  <si>
-    <t>CAD</t>
   </si>
   <si>
     <t>Logics - do not delete</t>
@@ -572,11 +549,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -584,7 +561,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -613,11 +590,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -653,13 +625,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -693,7 +665,7 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-9.9978637043366805E-2"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -876,9 +848,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -892,15 +864,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -911,7 +883,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="10" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -930,38 +902,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -976,10 +936,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -988,7 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1000,34 +960,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1305,21 +1265,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A061C73F-1F33-4614-90A5-D5D9D7C58056}">
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:F29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="8" customWidth="1"/>
-    <col min="2" max="2" width="47.83203125" style="8" customWidth="1"/>
-    <col min="3" max="6" width="20.83203125" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="8"/>
+    <col min="1" max="1" width="2.46484375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="47.796875" style="8" customWidth="1"/>
+    <col min="3" max="6" width="20.796875" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="8.796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>62</v>
@@ -1337,7 +1297,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6">
       <c r="B3" s="8" t="s">
         <v>61</v>
       </c>
@@ -1352,7 +1312,7 @@
       </c>
       <c r="F3" s="14"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6">
       <c r="B4" s="8" t="s">
         <v>65</v>
       </c>
@@ -1365,7 +1325,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="14.25" thickBot="1">
       <c r="B5" s="25" t="s">
         <v>66</v>
       </c>
@@ -1376,7 +1336,7 @@
       <c r="E5" s="20"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="14.25" thickTop="1">
       <c r="B6" s="7" t="s">
         <v>116</v>
       </c>
@@ -1385,16 +1345,16 @@
         <v>0.06</v>
       </c>
       <c r="D6" s="21">
-        <f>MAX(D4,C6*1.2)</f>
-        <v>7.1999999999999995E-2</v>
+        <f>MAX(D4,C6*1.15)</f>
+        <v>6.8999999999999992E-2</v>
       </c>
       <c r="E6" s="21">
         <f>(C6+D6)/2</f>
-        <v>6.6000000000000003E-2</v>
+        <v>6.4500000000000002E-2</v>
       </c>
       <c r="F6" s="21"/>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>77</v>
@@ -1403,7 +1363,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6">
       <c r="B10" s="8" t="s">
         <v>93</v>
       </c>
@@ -1412,10 +1372,10 @@
       </c>
       <c r="E10" s="27"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6">
       <c r="E11" s="27"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6">
       <c r="B12" s="4" t="s">
         <v>75</v>
       </c>
@@ -1423,7 +1383,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6">
       <c r="B13" s="4" t="s">
         <v>64</v>
       </c>
@@ -1431,7 +1391,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6">
       <c r="B15" s="4" t="s">
         <v>70</v>
       </c>
@@ -1439,7 +1399,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6">
       <c r="B16" s="4" t="s">
         <v>71</v>
       </c>
@@ -1447,7 +1407,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:6">
       <c r="B17" s="4" t="s">
         <v>72</v>
       </c>
@@ -1455,133 +1415,88 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B20" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="C20" s="32">
-        <v>1</v>
-      </c>
-      <c r="D20" s="31">
-        <v>2.1309999999999999E-2</v>
-      </c>
-      <c r="E20" s="30">
-        <v>2.7650000000000001E-2</v>
-      </c>
-      <c r="F20" s="31"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B21" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="33">
-        <v>1</v>
-      </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B22" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32">
-        <v>1</v>
-      </c>
-      <c r="F22" s="31"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B24" s="6" t="s">
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="B20" s="6" t="s">
         <v>89</v>
       </c>
+      <c r="C20" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="B22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="B23" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" s="8" t="s">
+        <v>100</v>
+      </c>
       <c r="C24" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B26" s="6" t="s">
-        <v>92</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="B26" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B27" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="B27" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B28" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B30" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B31" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C31" s="26" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.15">
-      <c r="B33" s="8" t="s">
+    <row r="29" spans="1:6">
+      <c r="B29" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C29" s="26" t="s">
         <v>108</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C17" r:id="rId1" xr:uid="{DB671679-E839-B64A-AD4E-6D8A323DAFC3}"/>
     <hyperlink ref="C16" r:id="rId2" xr:uid="{9CB8AD70-9E02-9A41-8E3A-990A0C1E81AE}"/>
     <hyperlink ref="C15" r:id="rId3" xr:uid="{45D5643F-FA1A-3C48-B2D9-4B6082295A37}"/>
     <hyperlink ref="C13" r:id="rId4" xr:uid="{35ACA25B-AF93-B04F-A9DD-9D3D634DC7A6}"/>
     <hyperlink ref="C12" r:id="rId5" xr:uid="{8FF27AF7-25A6-F443-A0E6-DAC1AFC8FB4A}"/>
-    <hyperlink ref="C24" r:id="rId6" xr:uid="{16104B09-A651-7A41-A777-F49F69D02554}"/>
-    <hyperlink ref="C26" r:id="rId7" xr:uid="{BFEB5D28-D16E-9545-989F-F86E412707A9}"/>
+    <hyperlink ref="C20" r:id="rId6" xr:uid="{16104B09-A651-7A41-A777-F49F69D02554}"/>
+    <hyperlink ref="C22" r:id="rId7" xr:uid="{BFEB5D28-D16E-9545-989F-F86E412707A9}"/>
     <hyperlink ref="C10" r:id="rId8" xr:uid="{E414D4D1-755D-2A43-AB81-B4A0517E9107}"/>
-    <hyperlink ref="C28" r:id="rId9" xr:uid="{645528C6-7225-564E-908E-A85650E1CCD6}"/>
-    <hyperlink ref="C27" r:id="rId10" xr:uid="{0B036CAC-824D-E543-8C48-9EDDC7350EA2}"/>
-    <hyperlink ref="C30" r:id="rId11" xr:uid="{EF5F9EA6-9DD5-1C42-A0E5-61DBB0A5A02F}"/>
-    <hyperlink ref="C31" r:id="rId12" xr:uid="{1DE792CC-A9C9-BB47-A69A-D22E477A4A3B}"/>
-    <hyperlink ref="C33" r:id="rId13" xr:uid="{E7131674-9823-C34D-8EBB-49D25F896885}"/>
+    <hyperlink ref="C24" r:id="rId9" xr:uid="{645528C6-7225-564E-908E-A85650E1CCD6}"/>
+    <hyperlink ref="C23" r:id="rId10" xr:uid="{0B036CAC-824D-E543-8C48-9EDDC7350EA2}"/>
+    <hyperlink ref="C26" r:id="rId11" xr:uid="{EF5F9EA6-9DD5-1C42-A0E5-61DBB0A5A02F}"/>
+    <hyperlink ref="C27" r:id="rId12" xr:uid="{1DE792CC-A9C9-BB47-A69A-D22E477A4A3B}"/>
+    <hyperlink ref="C29" r:id="rId13" xr:uid="{E7131674-9823-C34D-8EBB-49D25F896885}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId14"/>
@@ -1592,82 +1507,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB43275-BEC1-4DF6-B56D-B5F180583A40}">
   <dimension ref="A2:F70"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="1" max="1" width="2.5" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" customWidth="1"/>
-    <col min="3" max="6" width="20.83203125" customWidth="1"/>
+    <col min="1" max="1" width="2.46484375" customWidth="1"/>
+    <col min="2" max="2" width="41.796875" customWidth="1"/>
+    <col min="3" max="6" width="20.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="57" t="s">
-        <v>128</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="6" t="s">
-        <v>127</v>
-      </c>
       <c r="C4" s="16" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="B5" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="57" t="s">
-        <v>125</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="B7" s="53" t="s">
+        <v>121</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="B9" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
-      <c r="F11" s="58"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="54"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="8"/>
       <c r="B12" s="4" t="s">
         <v>95</v>
@@ -1679,12 +1594,12 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="8"/>
       <c r="B14" s="4" t="s">
         <v>98</v>
@@ -1695,7 +1610,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="8"/>
       <c r="B15" s="6" t="s">
         <v>56</v>
@@ -1706,7 +1621,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="8"/>
       <c r="B16" s="6" t="s">
         <v>57</v>
@@ -1717,7 +1632,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="B17" s="6" t="s">
         <v>58</v>
       </c>
@@ -1725,120 +1640,120 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" s="53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B20" s="57" t="s">
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" s="53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B26" s="57" t="s">
+    <row r="27" spans="1:3">
+      <c r="B27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28" t="s">
         <v>131</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C28" s="16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="16" t="s">
+      <c r="C29" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>136</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>137</v>
-      </c>
       <c r="C30" s="16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15">
       <c r="A32" s="3"/>
       <c r="B32" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="B33" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="B34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="57" t="s">
+    <row r="35" spans="1:6">
+      <c r="B35" s="53" t="s">
+        <v>137</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="B36" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="57" t="s">
-        <v>145</v>
-      </c>
       <c r="C36" s="16" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15">
       <c r="A40" s="3"/>
       <c r="B40" s="12" t="s">
         <v>54</v>
@@ -1850,596 +1765,596 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" s="4"/>
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="46" t="s">
         <v>53</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="9"/>
       <c r="E41" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="4"/>
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="30">
         <f t="shared" ref="E42:F45" si="0">IF(LEFT(C42,1)="H",1,IF(LEFT(C42,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
-      <c r="F42" s="34">
+      <c r="F42" s="30">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" s="4"/>
-      <c r="B43" s="51" t="s">
+      <c r="B43" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="40" t="s">
+      <c r="C43" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E43" s="30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F43" s="34">
+      <c r="F43" s="30">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" s="4"/>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="41" t="s">
+      <c r="D44" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="E44" s="34">
+      <c r="E44" s="30">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="F44" s="34">
+      <c r="F44" s="30">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" s="4"/>
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="C45" s="42" t="s">
+      <c r="C45" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="34">
+      <c r="E45" s="30">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F45" s="34">
+      <c r="F45" s="30">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" s="4"/>
-      <c r="B46" s="53" t="s">
+      <c r="B46" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="43" t="str">
+      <c r="C46" s="39" t="str">
         <f>IF(SUM(E42:E45)&gt;=3, "Hot", IF(SUM(E42:E45)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Mixed</v>
       </c>
-      <c r="D46" s="43" t="str">
+      <c r="D46" s="39" t="str">
         <f>IF(SUM(F42:F45)&gt;=3, "Hot", IF(SUM(F42:F45)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E46" s="34">
+      <c r="E46" s="30">
         <f>IF(LEFT(C46,1)="H",2,IF(LEFT(C46,1)="C",-1,0))</f>
         <v>0</v>
       </c>
-      <c r="F46" s="34">
+      <c r="F46" s="30">
         <f>IF(LEFT(D46,1)="H",2,IF(LEFT(D46,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" s="4"/>
-      <c r="B47" s="51" t="s">
+      <c r="B47" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="39" t="s">
+      <c r="C47" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D47" s="39" t="s">
+      <c r="D47" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="34">
+      <c r="E47" s="30">
         <f t="shared" ref="E47:F50" si="1">IF(LEFT(C47,1)="H",1,IF(LEFT(C47,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
-      <c r="F47" s="34">
+      <c r="F47" s="30">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" s="4"/>
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="39" t="s">
+      <c r="C48" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="39" t="s">
+      <c r="D48" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E48" s="34">
+      <c r="E48" s="30">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="F48" s="34">
+      <c r="F48" s="30">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6">
       <c r="A49" s="4"/>
-      <c r="B49" s="51" t="s">
+      <c r="B49" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="42" t="s">
+      <c r="C49" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="42" t="s">
+      <c r="D49" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E49" s="34">
+      <c r="E49" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F49" s="34">
+      <c r="F49" s="30">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6">
       <c r="A50" s="4"/>
-      <c r="B50" s="51" t="s">
+      <c r="B50" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="42" t="s">
+      <c r="D50" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E50" s="34">
+      <c r="E50" s="30">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="F50" s="34">
+      <c r="F50" s="30">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6">
       <c r="A51" s="4"/>
-      <c r="B51" s="53" t="s">
+      <c r="B51" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C51" s="44" t="str">
+      <c r="C51" s="40" t="str">
         <f>IF(SUM(E47:E50)&gt;=3, "Hot", IF(SUM(E47:E50)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="D51" s="44" t="str">
+      <c r="D51" s="40" t="str">
         <f>IF(SUM(F47:F50)&gt;=3, "Hot", IF(SUM(F47:F50)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E51" s="34">
+      <c r="E51" s="30">
         <f>IF(LEFT(C51,1)="H",2,IF(LEFT(C51,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
-      <c r="F51" s="34">
+      <c r="F51" s="30">
         <f>IF(LEFT(D51,1)="H",2,IF(LEFT(D51,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="27.75">
       <c r="A52" s="4"/>
-      <c r="B52" s="51" t="s">
+      <c r="B52" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="C52" s="39" t="s">
+      <c r="C52" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D52" s="39" t="s">
+      <c r="D52" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E52" s="34">
+      <c r="E52" s="30">
         <f t="shared" ref="E52:F55" si="2">IF(LEFT(C52,1)="H",1,IF(LEFT(C52,1)="C",-1,0))</f>
         <v>1</v>
       </c>
-      <c r="F52" s="34">
+      <c r="F52" s="30">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6">
       <c r="A53" s="4"/>
-      <c r="B53" s="51" t="s">
+      <c r="B53" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D53" s="39" t="s">
+      <c r="D53" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E53" s="34">
+      <c r="E53" s="30">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F53" s="34">
+      <c r="F53" s="30">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6">
       <c r="A54" s="4"/>
-      <c r="B54" s="51" t="s">
+      <c r="B54" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="C54" s="39" t="s">
+      <c r="C54" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="39" t="s">
+      <c r="D54" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E54" s="34">
+      <c r="E54" s="30">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F54" s="34">
+      <c r="F54" s="30">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6">
       <c r="A55" s="4"/>
-      <c r="B55" s="51" t="s">
+      <c r="B55" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="C55" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="39" t="s">
+      <c r="D55" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="34">
+      <c r="E55" s="30">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F55" s="34">
+      <c r="F55" s="30">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" s="4"/>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="44" t="str">
+      <c r="C56" s="40" t="str">
         <f>IF(SUM(E52:E55)&gt;=3, "Hot", IF(SUM(E52:E55)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Mixed</v>
       </c>
-      <c r="D56" s="44" t="str">
+      <c r="D56" s="40" t="str">
         <f>IF(SUM(F52:F55)&gt;=3, "Hot", IF(SUM(F52:F55)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E56" s="34">
+      <c r="E56" s="30">
         <f>IF(LEFT(C56,1)="H",2,IF(LEFT(C56,1)="C",-1,0))</f>
         <v>0</v>
       </c>
-      <c r="F56" s="34">
+      <c r="F56" s="30">
         <f>IF(LEFT(D56,1)="H",2,IF(LEFT(D56,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="27.75">
       <c r="A57" s="4"/>
-      <c r="B57" s="51" t="s">
+      <c r="B57" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="39" t="s">
+      <c r="C57" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="D57" s="39" t="s">
+      <c r="D57" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E57" s="34">
+      <c r="E57" s="30">
         <f t="shared" ref="E57:F60" si="3">IF(LEFT(C57,1)="H",1,IF(LEFT(C57,1)="C",-1,0))</f>
         <v>0</v>
       </c>
-      <c r="F57" s="34">
+      <c r="F57" s="30">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="27.75">
       <c r="A58" s="4"/>
-      <c r="B58" s="51" t="s">
+      <c r="B58" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="39" t="s">
+      <c r="C58" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D58" s="39" t="s">
+      <c r="D58" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E58" s="34">
+      <c r="E58" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F58" s="34">
+      <c r="F58" s="30">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6">
       <c r="A59" s="4"/>
-      <c r="B59" s="51" t="s">
+      <c r="B59" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="39" t="s">
+      <c r="C59" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="D59" s="39" t="s">
+      <c r="D59" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E59" s="34">
+      <c r="E59" s="30">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="F59" s="34">
+      <c r="F59" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="27.75">
       <c r="A60" s="4"/>
-      <c r="B60" s="51" t="s">
+      <c r="B60" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C60" s="39" t="s">
+      <c r="C60" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="39" t="s">
+      <c r="D60" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E60" s="34">
+      <c r="E60" s="30">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="F60" s="34">
+      <c r="F60" s="30">
         <f t="shared" si="3"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" s="4"/>
-      <c r="B61" s="53" t="s">
+      <c r="B61" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="44" t="str">
+      <c r="C61" s="40" t="str">
         <f>IF(SUM(E57:E60)&gt;=3, "Hot", IF(SUM(E57:E60)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Mixed</v>
       </c>
-      <c r="D61" s="44" t="str">
+      <c r="D61" s="40" t="str">
         <f>IF(SUM(F57:F60)&gt;=3, "Hot", IF(SUM(F57:F60)&lt;=-3,"Cold", "Mixed"))</f>
         <v>Cold</v>
       </c>
-      <c r="E61" s="34">
+      <c r="E61" s="30">
         <f>IF(LEFT(C61,1)="H",2,IF(LEFT(C61,1)="C",-1,0))</f>
         <v>0</v>
       </c>
-      <c r="F61" s="34">
+      <c r="F61" s="30">
         <f>IF(LEFT(D61,1)="H",2,IF(LEFT(D61,1)="C",-1,0))</f>
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="27.75">
       <c r="A62" s="4"/>
-      <c r="B62" s="54" t="s">
+      <c r="B62" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="45" t="str">
+      <c r="C62" s="41" t="str">
         <f>IF(OR(E62=4,E62=-4),"In extreme",IF(E62=0,"In equilibrium",IF(OR(E62&gt;0),"Relatively optimistic","Relatively pessimistic")))</f>
         <v>Relatively pessimistic</v>
       </c>
-      <c r="D62" s="45" t="str">
+      <c r="D62" s="41" t="str">
         <f>IF(OR(F62=4,F62=-4),"In extreme",IF(F62=0,"In equilibrium",IF(OR(F62&gt;0),"Relatively optimistic","Relatively pessimistic")))</f>
         <v>In extreme</v>
       </c>
-      <c r="E62" s="35">
+      <c r="E62" s="31">
         <f>SUM(E46,E51,E56,E61)</f>
         <v>-1</v>
       </c>
-      <c r="F62" s="35">
+      <c r="F62" s="31">
         <f>SUM(F46,F51,F56,F61)</f>
         <v>-4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" s="4"/>
-      <c r="B63" s="46"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="46"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="4"/>
-      <c r="B64" s="55" t="s">
+      <c r="B64" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="47" t="s">
+      <c r="C64" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D64" s="47" t="s">
+      <c r="D64" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="E64" s="37"/>
-      <c r="F64" s="37"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E64" s="33"/>
+      <c r="F64" s="33"/>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="4"/>
-      <c r="B65" s="52" t="s">
+      <c r="B65" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="42" t="s">
+      <c r="C65" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="42" t="s">
+      <c r="D65" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="37">
+      <c r="E65" s="33">
         <f t="shared" ref="E65:F69" si="4">IF(LEFT(C65,1)="H",2,IF(LEFT(C65,1)="C",0,1))</f>
         <v>2</v>
       </c>
-      <c r="F65" s="37">
+      <c r="F65" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B66" s="52" t="s">
+    <row r="66" spans="1:6">
+      <c r="B66" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C66" s="48" t="e">
+      <c r="C66" s="44" t="e">
         <f>IF(Macro!#REF!&gt;=3%, "Hot - High", IF(Macro!#REF!&lt;=1.5%, "Cold - Low", "Mixed - Dormant"))</f>
         <v>#REF!</v>
       </c>
-      <c r="D66" s="48" t="e">
+      <c r="D66" s="44" t="e">
         <f>IF(Macro!#REF!&gt;=3%, "Hot - High", IF(Macro!#REF!&lt;=1.5%, "Cold - Low", "Mixed - Dormant"))</f>
         <v>#REF!</v>
       </c>
-      <c r="E66" s="37" t="e">
+      <c r="E66" s="33" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
-      <c r="F66" s="37" t="e">
+      <c r="F66" s="33" t="e">
         <f t="shared" si="4"/>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B67" s="52" t="s">
+    <row r="67" spans="1:6">
+      <c r="B67" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C67" s="48" t="str">
+      <c r="C67" s="44" t="str">
         <f>C43</f>
         <v>Hot - Positive</v>
       </c>
-      <c r="D67" s="48" t="str">
+      <c r="D67" s="44" t="str">
         <f>D43</f>
         <v>Cold - Negative</v>
       </c>
-      <c r="E67" s="37">
+      <c r="E67" s="33">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F67" s="37">
+      <c r="F67" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B68" s="52" t="s">
+    <row r="68" spans="1:6">
+      <c r="B68" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C68" s="48" t="str">
+      <c r="C68" s="44" t="str">
         <f>C49</f>
         <v>Mixed</v>
       </c>
-      <c r="D68" s="48" t="str">
+      <c r="D68" s="44" t="str">
         <f>D49</f>
         <v>Cold - High</v>
       </c>
-      <c r="E68" s="37">
+      <c r="E68" s="33">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="F68" s="37">
+      <c r="F68" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B69" s="52" t="s">
+    <row r="69" spans="1:6">
+      <c r="B69" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="48" t="str">
+      <c r="C69" s="44" t="str">
         <f>C50</f>
         <v>Cold - Wide</v>
       </c>
-      <c r="D69" s="48" t="str">
+      <c r="D69" s="44" t="str">
         <f>D50</f>
         <v>Cold - Wide</v>
       </c>
-      <c r="E69" s="37">
+      <c r="E69" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F69" s="37">
+      <c r="F69" s="33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B70" s="56" t="s">
+    <row r="70" spans="1:6">
+      <c r="B70" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C70" s="49" t="e">
+      <c r="C70" s="45" t="e">
         <f>Macro!#REF!*(1+E70)</f>
         <v>#REF!</v>
       </c>
-      <c r="D70" s="49" t="e">
+      <c r="D70" s="45" t="e">
         <f>Macro!#REF!*(1+F70)</f>
         <v>#REF!</v>
       </c>
-      <c r="E70" s="38" t="e">
+      <c r="E70" s="34" t="e">
         <f>SUM(E65:E69)/10</f>
         <v>#REF!</v>
       </c>
-      <c r="F70" s="38" t="e">
+      <c r="F70" s="34" t="e">
         <f>SUM(F65:F69)/10</f>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations count="19">
     <dataValidation allowBlank="1" sqref="C62:D62" xr:uid="{EA6F9DE9-1D2B-41CE-B86F-59C772E5B0CA}"/>
     <dataValidation type="list" allowBlank="1" sqref="C49:D49" xr:uid="{CB91B3B3-F107-40CA-9A38-987E11E74D07}">
@@ -2531,21 +2446,21 @@
       <selection activeCell="B2" sqref="B2:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.9"/>
   <cols>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3">
       <c r="B2" s="15" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
       <c r="B4" s="15" t="s">
         <v>84</v>
       </c>
@@ -2553,12 +2468,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3">
       <c r="B6" s="15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
         <v>78</v>
       </c>
@@ -2566,12 +2481,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3">
       <c r="B9" s="22" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3">
       <c r="B10" t="s">
         <v>81</v>
       </c>
@@ -2579,12 +2494,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3">
       <c r="B12" s="15" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>87</v>
       </c>
@@ -2593,7 +2508,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1" xr:uid="{BD2948D7-96D9-264F-B0D8-E6D98C96444B}"/>
     <hyperlink ref="C10" r:id="rId2" xr:uid="{00B87B71-2B64-7648-8C06-ED4B13CF1CAC}"/>
@@ -2613,14 +2528,14 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="34.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4">
       <c r="C2" s="1" t="s">
         <v>114</v>
       </c>
@@ -2628,7 +2543,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -2636,33 +2551,33 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4">
       <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4">
       <c r="B7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4">
       <c r="B9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:4">
       <c r="B11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:4">
       <c r="B13" t="s">
         <v>113</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{D5EB599C-0AC8-C945-97CD-4616A9DA5B5A}"/>
   </hyperlinks>

</xml_diff>